<commit_message>
Worked on alternative solver, fixed some bugs.
</commit_message>
<xml_diff>
--- a/misc/performance_test.xlsx
+++ b/misc/performance_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Google Drive\Scripts\GitHub\plasma-solver\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DE1AD-13DC-458D-9D33-28122AE6AF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C081D8-FF96-4E69-A0EE-A277F4CBC95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F8CC7C9-630F-4D37-82F0-443335F1FF8A}"/>
+    <workbookView xWindow="22920" yWindow="3555" windowWidth="10455" windowHeight="11325" xr2:uid="{7F8CC7C9-630F-4D37-82F0-443335F1FF8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>nLoops</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>No negative velocity, double radial resolution</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Execution</t>
   </si>
 </sst>
 </file>
@@ -113,12 +119,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,6 +933,428 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$34:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9999999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9999999999999999E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9999999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9999999999999998E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9999999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9999999999999997E-7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9999999999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$34:$B$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.5224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.394200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.560200000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.441800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>124.9239</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>157.35730000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>189.81219999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>226.3047</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>267.63049999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>310.07589999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>353.2328</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>394.33890000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>436.13080000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>478.3263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DAD3-40F2-9ADD-5A9206A8D3DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="431134288"/>
+        <c:axId val="431134616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="431134288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431134616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="431134616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431134288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1006,6 +1435,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1523,6 +1992,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2292,6 +3277,42 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>184149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>275167</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>69849</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F501C4C-F7E9-4D4D-BC93-BB6AEEFA56E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2594,12 +3615,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8323124F-07D5-4333-BE9A-B272557E5E52}">
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="14" max="14" width="20.85546875" customWidth="1"/>
     <col min="15" max="15" width="15.28515625" customWidth="1"/>
@@ -2654,11 +3676,11 @@
         <v>96.38768665147802</v>
       </c>
       <c r="N3" s="1">
-        <f>M3/60</f>
+        <f t="shared" ref="N3:O5" si="0">M3/60</f>
         <v>1.6064614441913003</v>
       </c>
       <c r="O3" s="1">
-        <f>N3/60</f>
+        <f t="shared" si="0"/>
         <v>2.6774357403188339E-2</v>
       </c>
       <c r="P3" s="1">
@@ -2670,7 +3692,7 @@
         <v>1.5937117501897821E-4</v>
       </c>
       <c r="R3" s="1">
-        <f>P3/365.25</f>
+        <f t="shared" ref="R3:R10" si="1">P3/365.25</f>
         <v>3.0543414788031414E-6</v>
       </c>
     </row>
@@ -2686,15 +3708,15 @@
         <v>1000000</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M10" si="0">93.539*EXP(0.0000003*L4)</f>
+        <f t="shared" ref="M4:M10" si="2">93.539*EXP(0.0000003*L4)</f>
         <v>126.26444300185176</v>
       </c>
       <c r="N4" s="1">
-        <f>M4/60</f>
+        <f t="shared" si="0"/>
         <v>2.1044073833641961</v>
       </c>
       <c r="O4" s="1">
-        <f>N4/60</f>
+        <f t="shared" si="0"/>
         <v>3.5073456389403269E-2</v>
       </c>
       <c r="P4" s="1">
@@ -2706,7 +3728,7 @@
         <v>2.0877057374644802E-4</v>
       </c>
       <c r="R4" s="1">
-        <f>P4/365.25</f>
+        <f t="shared" si="1"/>
         <v>4.0010787576321318E-6</v>
       </c>
     </row>
@@ -2721,15 +3743,15 @@
         <v>5000000</v>
       </c>
       <c r="M5" s="2">
+        <f t="shared" si="2"/>
+        <v>419.21271395035222</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>419.21271395035222</v>
-      </c>
-      <c r="N5" s="1">
-        <f>M5/60</f>
         <v>6.9868785658392039</v>
       </c>
       <c r="O5" s="1">
-        <f>N5/60</f>
+        <f t="shared" si="0"/>
         <v>0.11644797609732006</v>
       </c>
       <c r="P5" s="1">
@@ -2741,7 +3763,7 @@
         <v>6.9314271486500042E-4</v>
       </c>
       <c r="R5" s="1">
-        <f>P5/365.25</f>
+        <f t="shared" si="1"/>
         <v>1.3284049292416161E-5</v>
       </c>
     </row>
@@ -2757,27 +3779,27 @@
         <v>10000000</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1878.7810382580512</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:O8" si="1">M6/60</f>
+        <f t="shared" ref="N6:O8" si="3">M6/60</f>
         <v>31.313017304300853</v>
       </c>
       <c r="O6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.52188362173834757</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" ref="P6:P8" si="4">O6/24</f>
+        <v>2.1745150905764482E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ref="Q6:Q8" si="5">P6/7</f>
+        <v>3.1064501293949259E-3</v>
+      </c>
+      <c r="R6" s="1">
         <f t="shared" si="1"/>
-        <v>0.52188362173834757</v>
-      </c>
-      <c r="P6" s="1">
-        <f t="shared" ref="P6:P8" si="2">O6/24</f>
-        <v>2.1745150905764482E-2</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" ref="Q6:Q8" si="3">P6/7</f>
-        <v>3.1064501293949259E-3</v>
-      </c>
-      <c r="R6" s="1">
-        <f>P6/365.25</f>
         <v>5.9534978523653615E-5</v>
       </c>
     </row>
@@ -2793,27 +3815,27 @@
         <v>20000000</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>37736.32591451695</v>
       </c>
       <c r="N7" s="1">
+        <f t="shared" si="3"/>
+        <v>628.93876524194923</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="3"/>
+        <v>10.482312754032487</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="4"/>
+        <v>0.43676303141802025</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="5"/>
+        <v>6.2394718774002891E-2</v>
+      </c>
+      <c r="R7" s="1">
         <f t="shared" si="1"/>
-        <v>628.93876524194923</v>
-      </c>
-      <c r="O7" s="1">
-        <f t="shared" si="1"/>
-        <v>10.482312754032487</v>
-      </c>
-      <c r="P7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.43676303141802025</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="3"/>
-        <v>6.2394718774002891E-2</v>
-      </c>
-      <c r="R7" s="1">
-        <f>P7/365.25</f>
         <v>1.1957920093580295E-3</v>
       </c>
     </row>
@@ -2829,27 +3851,27 @@
         <v>30000000</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>757954.36750147387</v>
       </c>
       <c r="N8" s="1">
+        <f t="shared" si="3"/>
+        <v>12632.572791691231</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="3"/>
+        <v>210.5428798615205</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="4"/>
+        <v>8.7726199942300216</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2532314277471459</v>
+      </c>
+      <c r="R8" s="1">
         <f t="shared" si="1"/>
-        <v>12632.572791691231</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" si="1"/>
-        <v>210.5428798615205</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="2"/>
-        <v>8.7726199942300216</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="3"/>
-        <v>1.2532314277471459</v>
-      </c>
-      <c r="R8" s="1">
-        <f>P8/365.25</f>
         <v>2.4018124556413476E-2</v>
       </c>
     </row>
@@ -2865,7 +3887,7 @@
         <v>50000000</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>305780616.00366879</v>
       </c>
       <c r="N9" s="1">
@@ -2885,7 +3907,7 @@
         <v>505.58964286320901</v>
       </c>
       <c r="R9" s="1">
-        <f>P9/365.25</f>
+        <f t="shared" si="1"/>
         <v>9.6896030117521228</v>
       </c>
     </row>
@@ -2901,7 +3923,7 @@
         <v>100000000</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>999602145881216.75</v>
       </c>
       <c r="N10" s="1">
@@ -2909,7 +3931,7 @@
         <v>16660035764686.945</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" ref="O10" si="4">N10/60</f>
+        <f t="shared" ref="O10" si="6">N10/60</f>
         <v>277667262744.78241</v>
       </c>
       <c r="P10" s="1">
@@ -2921,7 +3943,7 @@
         <v>1652781325.8618</v>
       </c>
       <c r="R10" s="1">
-        <f>P10/365.25</f>
+        <f t="shared" si="1"/>
         <v>31675480.577775773</v>
       </c>
     </row>
@@ -3003,11 +4025,11 @@
         <v>107.43825081604301</v>
       </c>
       <c r="N18" s="3">
-        <f>M18/60</f>
+        <f t="shared" ref="N18:O20" si="7">M18/60</f>
         <v>1.7906375136007169</v>
       </c>
       <c r="O18" s="1">
-        <f>N18/60</f>
+        <f t="shared" si="7"/>
         <v>2.9843958560011947E-2</v>
       </c>
       <c r="P18" s="1">
@@ -3019,7 +4041,7 @@
         <v>1.7764261047626157E-4</v>
       </c>
       <c r="R18" s="4">
-        <f>P18/365.25</f>
+        <f t="shared" ref="R18:R25" si="8">P18/365.25</f>
         <v>3.4045127264444382E-6</v>
       </c>
     </row>
@@ -3033,11 +4055,11 @@
         <v>649.9635416302367</v>
       </c>
       <c r="N19" s="3">
-        <f>M19/60</f>
+        <f t="shared" si="7"/>
         <v>10.832725693837279</v>
       </c>
       <c r="O19" s="1">
-        <f>N19/60</f>
+        <f t="shared" si="7"/>
         <v>0.18054542823062131</v>
       </c>
       <c r="P19" s="1">
@@ -3049,7 +4071,7 @@
         <v>1.0746751680394124E-3</v>
       </c>
       <c r="R19" s="4">
-        <f>P19/365.25</f>
+        <f t="shared" si="8"/>
         <v>2.05961017830962E-5</v>
       </c>
     </row>
@@ -3058,15 +4080,15 @@
         <v>5000000</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" ref="M20:M25" si="5">87.963*EXP(0.000002*L20)</f>
+        <f t="shared" ref="M20:M25" si="9">87.963*EXP(0.000002*L20)</f>
         <v>1937514.0107085833</v>
       </c>
       <c r="N20" s="3">
-        <f>M20/60</f>
+        <f t="shared" si="7"/>
         <v>32291.90017847639</v>
       </c>
       <c r="O20" s="1">
-        <f>N20/60</f>
+        <f t="shared" si="7"/>
         <v>538.19833630793983</v>
       </c>
       <c r="P20" s="1">
@@ -3078,7 +4100,7 @@
         <v>3.203561525642499</v>
       </c>
       <c r="R20" s="4">
-        <f>P20/365.25</f>
+        <f t="shared" si="8"/>
         <v>6.139611411224502E-2</v>
       </c>
     </row>
@@ -3088,27 +4110,27 @@
         <v>10000000</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>42676586083.831383</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" ref="N21:O21" si="6">M21/60</f>
+        <f t="shared" ref="N21:O21" si="10">M21/60</f>
         <v>711276434.73052299</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>11854607.245508717</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" ref="P21:P23" si="7">O21/24</f>
+        <f t="shared" ref="P21:P23" si="11">O21/24</f>
         <v>493941.96856286324</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" ref="Q21:Q23" si="8">P21/7</f>
+        <f t="shared" ref="Q21:Q23" si="12">P21/7</f>
         <v>70563.138366123327</v>
       </c>
       <c r="R21" s="4">
-        <f>P21/365.25</f>
+        <f t="shared" si="8"/>
         <v>1352.3394074274147</v>
       </c>
     </row>
@@ -3118,27 +4140,27 @@
         <v>20000000</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.0705194226784788E+19</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" ref="N22:O22" si="9">M22/60</f>
+        <f t="shared" ref="N22:O22" si="13">M22/60</f>
         <v>3.4508657044641312E+17</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>5751442840773552</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>239643451698898</v>
       </c>
       <c r="Q22" s="1">
+        <f t="shared" si="12"/>
+        <v>34234778814128.285</v>
+      </c>
+      <c r="R22" s="4">
         <f t="shared" si="8"/>
-        <v>34234778814128.285</v>
-      </c>
-      <c r="R22" s="4">
-        <f>P22/365.25</f>
         <v>656108012864.88159</v>
       </c>
     </row>
@@ -3148,27 +4170,27 @@
         <v>30000000</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.0045439603035702E+28</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" ref="N23:O23" si="10">M23/60</f>
+        <f t="shared" ref="N23:O23" si="14">M23/60</f>
         <v>1.6742399338392835E+26</v>
       </c>
       <c r="O23" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.790399889732139E+24</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.1626666207217245E+23</v>
       </c>
       <c r="Q23" s="1">
+        <f t="shared" si="12"/>
+        <v>1.6609523153167492E+22</v>
+      </c>
+      <c r="R23" s="4">
         <f t="shared" si="8"/>
-        <v>1.6609523153167492E+22</v>
-      </c>
-      <c r="R23" s="4">
-        <f>P23/365.25</f>
         <v>3.1832077227151937E+20</v>
       </c>
     </row>
@@ -3178,7 +4200,7 @@
         <v>50000000</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.3645484814557271E+45</v>
       </c>
       <c r="N24" s="3">
@@ -3198,7 +4220,7 @@
         <v>3.9096370394439933E+39</v>
       </c>
       <c r="R24" s="4">
-        <f>P24/365.25</f>
+        <f t="shared" si="8"/>
         <v>7.4928019920897886E+37</v>
       </c>
     </row>
@@ -3208,7 +4230,7 @@
         <v>100000000</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.3561833056564522E+88</v>
       </c>
       <c r="N25" s="3">
@@ -3216,7 +4238,7 @@
         <v>1.0593638842760754E+87</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" ref="O25" si="11">N25/60</f>
+        <f t="shared" ref="O25" si="15">N25/60</f>
         <v>1.7656064737934591E+85</v>
       </c>
       <c r="P25" s="1">
@@ -3228,7 +4250,7 @@
         <v>1.0509562344008684E+83</v>
       </c>
       <c r="R25" s="4">
-        <f>P25/365.25</f>
+        <f t="shared" si="8"/>
         <v>2.0141529475170647E+81</v>
       </c>
     </row>
@@ -3237,9 +4259,148 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <f>0.0000001</f>
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B34">
+        <v>1.5224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <f>0.0000002</f>
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="B35">
+        <v>5.3148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>2.9999999999999999E-7</v>
+      </c>
+      <c r="B36">
+        <v>26.394200000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="B37">
+        <v>57.560200000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="B38">
+        <v>88.441800000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="B39">
+        <v>124.9239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="B40">
+        <v>157.35730000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>7.9999999999999996E-7</v>
+      </c>
+      <c r="B41">
+        <v>189.81219999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="B42">
+        <v>226.3047</v>
+      </c>
       <c r="L42" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B43">
+        <v>267.63049999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>1.1000000000000001E-6</v>
+      </c>
+      <c r="B44">
+        <v>310.07589999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>1.1999999999999999E-6</v>
+      </c>
+      <c r="B45">
+        <v>353.2328</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>1.3E-6</v>
+      </c>
+      <c r="B46">
+        <v>394.33890000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>1.3999999999999999E-6</v>
+      </c>
+      <c r="B47">
+        <v>436.13080000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>1.5E-6</v>
+      </c>
+      <c r="B48">
+        <v>478.3263</v>
+      </c>
+      <c r="C48" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D48">
+        <f>90000000000000*C48^2+200000000*C48-34.611</f>
+        <v>10965.389000000001</v>
+      </c>
+      <c r="E48">
+        <f>D48/60/60</f>
+        <v>3.0459413888888895</v>
       </c>
     </row>
     <row r="57" spans="12:12" x14ac:dyDescent="0.25">

</xml_diff>